<commit_message>
tambahkan fitur upload gambar di halaman edit tamu
</commit_message>
<xml_diff>
--- a/Laporan Buku Tamu.xlsx
+++ b/Laporan Buku Tamu.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
   <si>
     <t>No</t>
   </si>
@@ -86,94 +86,64 @@
     <t>Projek TEFA</t>
   </si>
   <si>
-    <t>2024-09-05</t>
+    <t>2025-09-06</t>
+  </si>
+  <si>
+    <t>Adit</t>
+  </si>
+  <si>
+    <t>Gg. Pangrango</t>
+  </si>
+  <si>
+    <t>0988348224</t>
+  </si>
+  <si>
+    <t>Pak Fajar</t>
+  </si>
+  <si>
+    <t>Remedial</t>
+  </si>
+  <si>
+    <t>Deryl</t>
+  </si>
+  <si>
+    <t>0988344353</t>
+  </si>
+  <si>
+    <t>Ibnu</t>
+  </si>
+  <si>
+    <t>Gg. Guntur 1</t>
+  </si>
+  <si>
+    <t>09883483564</t>
+  </si>
+  <si>
+    <t>2025-09-07</t>
   </si>
   <si>
     <t>Sion</t>
   </si>
   <si>
-    <t>Ikebukuro</t>
-  </si>
-  <si>
-    <t>098788232342</t>
+    <t>Jl. Suroso no 58</t>
+  </si>
+  <si>
+    <t>0884853833</t>
+  </si>
+  <si>
+    <t>Rofi</t>
+  </si>
+  <si>
+    <t>Bojong</t>
+  </si>
+  <si>
+    <t>0878128700</t>
   </si>
   <si>
     <t>Albert</t>
   </si>
   <si>
     <t>Pribadi</t>
-  </si>
-  <si>
-    <t>2025-09-06</t>
-  </si>
-  <si>
-    <t>Adit</t>
-  </si>
-  <si>
-    <t>Gg. Pangrango</t>
-  </si>
-  <si>
-    <t>0988348224</t>
-  </si>
-  <si>
-    <t>Pak Fajar</t>
-  </si>
-  <si>
-    <t>Remedial</t>
-  </si>
-  <si>
-    <t>Deryl</t>
-  </si>
-  <si>
-    <t>0988344353</t>
-  </si>
-  <si>
-    <t>Ibnu</t>
-  </si>
-  <si>
-    <t>Gg. Guntur 1</t>
-  </si>
-  <si>
-    <t>09883483564</t>
-  </si>
-  <si>
-    <t>2025-09-07</t>
-  </si>
-  <si>
-    <t>Jl. Suroso no 58</t>
-  </si>
-  <si>
-    <t>0884853833</t>
-  </si>
-  <si>
-    <t>Rofi</t>
-  </si>
-  <si>
-    <t>Bojong</t>
-  </si>
-  <si>
-    <t>0878128700</t>
-  </si>
-  <si>
-    <t>JL. otto iskandar dinata 1</t>
-  </si>
-  <si>
-    <t>Jakarta</t>
-  </si>
-  <si>
-    <t>0884089087</t>
-  </si>
-  <si>
-    <t>Bu Sarah</t>
-  </si>
-  <si>
-    <t>Rafa</t>
-  </si>
-  <si>
-    <t>Warungkondang</t>
-  </si>
-  <si>
-    <t>Pak Yayat</t>
   </si>
 </sst>
 </file>
@@ -513,7 +483,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -638,22 +608,22 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" t="s">
         <v>29</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" t="s">
         <v>30</v>
       </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" t="s">
-        <v>32</v>
-      </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -661,22 +631,22 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -684,22 +654,22 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" t="s">
         <v>37</v>
       </c>
-      <c r="D8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" t="s">
-        <v>39</v>
-      </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -707,114 +677,22 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
         <v>40</v>
       </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="F9" t="s">
         <v>41</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>42</v>
-      </c>
-      <c r="F9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" t="s">
-        <v>49</v>
-      </c>
-      <c r="G12" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" t="s">
-        <v>52</v>
-      </c>
-      <c r="G13" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>